<commit_message>
Implementacion en Java, Analisis Big-O, Evaluacion Experimental
</commit_message>
<xml_diff>
--- a/Evaluacion_Experimental_Algortimo.xlsx
+++ b/Evaluacion_Experimental_Algortimo.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upbeduco-my.sharepoint.com/personal/thomas_vanegasa_upb_edu_co/Documents/ingenieria_sistemas_informatica_upb/semestre_5/estructuras_datos_algoritmos/Taller3-ThomasVanegas-AlejandroGomez/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="204" documentId="11_AD4D2F04E46CFB4ACB3E20AE8556C86A683EDF16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B067BE3-1605-4C49-8F42-D1AFCD6B48CD}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,22 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>EVALUACION EXPERIMENTAL MERGESORT USANDO LISTAS DOBLEMENTE ENLAZADAS</t>
+  </si>
+  <si>
+    <t>TIEMPO (ExecTimeSec)</t>
+  </si>
+  <si>
+    <t>LONGITUD DE LA LISTA ENLAZADA (N)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +65,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +109,986 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>Evaluación Experimental de MergeSort usando Listas Doblemente Enlazadas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$4:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$4:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>9.1299999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9199999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.37E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.435</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.562000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AB7D-427B-A85E-63728390D34B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1277221248"/>
+        <c:axId val="1277198688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1277221248"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="96000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1277198688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1277198688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1277221248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>239711</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>115886</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Gráfico 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FA28B54-B04E-2105-6316-C207B9AF0148}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +1353,232 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>9.1299999999999997E-5</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>100</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5.9199999999999997E-4</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>500</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2.1900000000000001E-3</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>5000</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.37E-2</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>10000</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B10" s="4">
+        <v>6.8400000000000002E-2</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>100000</v>
+      </c>
+      <c r="B11" s="4">
+        <v>9.2100000000000001E-2</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>500000</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.435</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="B14" s="4">
+        <v>6.22</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="B15" s="4">
+        <v>18.562000000000001</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>